<commit_message>
feat(matriz-adjacencia-ponderado): cria matriz de adjacencias para grafo ponderado
</commit_message>
<xml_diff>
--- a/grafo.xlsx
+++ b/grafo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laras\Desktop\trabalho de grafos\trabalho-grafos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tailine\Documents\7 Semestre\Teoria dos Grafos\trabalho-parte1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471436FE-DD5C-4F67-9219-39CBDB506381}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53428F4-93B3-47CD-94BD-B4ACFD2E36FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{CAB3AF3A-231C-4761-B78B-B90B909FA2BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7550" activeTab="1" xr2:uid="{CAB3AF3A-231C-4761-B78B-B90B909FA2BA}"/>
   </bookViews>
   <sheets>
     <sheet name="vertice" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>A</t>
   </si>
@@ -49,45 +49,6 @@
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>S</t>
   </si>
   <si>
     <t>AB</t>
@@ -454,107 +415,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD824F2-46FF-4DF3-B770-702D106B5BA2}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -567,14 +463,14 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -586,9 +482,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -600,9 +496,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -614,9 +510,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -625,12 +521,12 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
feat(matriz-adjacencia): cria matriz de adjacencia para grafo dirigido e não ponderado, e para grafo nao dirigido e nao ponderado
</commit_message>
<xml_diff>
--- a/grafo.xlsx
+++ b/grafo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tailine\Documents\7 Semestre\Teoria dos Grafos\trabalho-parte1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53428F4-93B3-47CD-94BD-B4ACFD2E36FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0164D1-B3C2-4252-A089-5B3806EA2A42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7550" activeTab="1" xr2:uid="{CAB3AF3A-231C-4761-B78B-B90B909FA2BA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>A</t>
   </si>
@@ -45,12 +45,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>AB</t>
   </si>
   <si>
@@ -60,10 +54,13 @@
     <t>BC</t>
   </si>
   <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>FA</t>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>DC</t>
   </si>
 </sst>
 </file>
@@ -415,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD824F2-46FF-4DF3-B770-702D106B5BA2}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -441,16 +438,6 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -460,17 +447,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5FBE10-4AF7-4748-81A8-9F1F1C4A7ABA}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -479,26 +466,26 @@
         <v>1</v>
       </c>
       <c r="D1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -507,39 +494,53 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(matriz dirigido): tinha sido erroneamente corrigida para fazer matriz de incidencia; feat(matriz ponderada e dirigida)
</commit_message>
<xml_diff>
--- a/grafo.xlsx
+++ b/grafo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tailine\Documents\7 Semestre\Teoria dos Grafos\trabalho-parte1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laras\Desktop\trabalho-grafos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0164D1-B3C2-4252-A089-5B3806EA2A42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D5CDEE-9B18-4BCF-A2F7-2D3CD4F8D797}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7550" activeTab="1" xr2:uid="{CAB3AF3A-231C-4761-B78B-B90B909FA2BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{CAB3AF3A-231C-4761-B78B-B90B909FA2BA}"/>
   </bookViews>
   <sheets>
     <sheet name="vertice" sheetId="1" r:id="rId1"/>
@@ -418,24 +418,24 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -450,12 +450,12 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -480,10 +480,10 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -497,7 +497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -511,7 +511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -522,10 +522,10 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>

</xml_diff>